<commit_message>
Changed fonts on all but the shop
 - When using the new font, if you up the size by 20 it seems to keep it the same size as the "Liberation" font.
 - Also updated Gantt chart
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\CS383\Tower-of-Annihilation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D5F41B-43FF-4A0F-8BDC-6D749AAA762A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C95F1E4-9070-4D9B-9C5B-B58FC8E5FDAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Overhead" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2615,11 +2616,11 @@
       </c>
       <c r="D8" s="18">
         <f t="shared" si="8"/>
-        <v>5600</v>
+        <v>6600</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" si="9"/>
-        <v>6200</v>
+        <v>5200</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="17">
@@ -2628,11 +2629,11 @@
       </c>
       <c r="H8" s="18">
         <f>(Gantt!$C56)*100</f>
-        <v>1300</v>
+        <v>2300</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="10"/>
-        <v>4400</v>
+        <v>3400</v>
       </c>
       <c r="K8" s="17">
         <v>2000</v>
@@ -2679,11 +2680,11 @@
       </c>
       <c r="D9" s="28">
         <f>SUM(D4:D8)</f>
-        <v>33700</v>
+        <v>34700</v>
       </c>
       <c r="E9" s="29">
         <f>SUM(E4:E8)</f>
-        <v>21800</v>
+        <v>20800</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="20">
@@ -2692,11 +2693,11 @@
       </c>
       <c r="H9" s="21">
         <f>SUM(H4:H8)</f>
-        <v>10500</v>
+        <v>11500</v>
       </c>
       <c r="I9" s="22">
         <f>SUM(I4:I8)</f>
-        <v>14500</v>
+        <v>13500</v>
       </c>
       <c r="K9" s="20">
         <f>SUM(K4:K8)</f>
@@ -2752,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BK58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4113,6 +4114,9 @@
       <c r="B49">
         <v>5</v>
       </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
       <c r="D49" t="s">
         <v>18</v>
       </c>
@@ -4145,7 +4149,7 @@
         <v>5</v>
       </c>
       <c r="C50">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D50" s="56" t="s">
         <v>18</v>
@@ -4183,7 +4187,7 @@
         <v>10</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
         <v>17</v>
@@ -4273,6 +4277,9 @@
       </c>
       <c r="B54">
         <v>5</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
       </c>
       <c r="D54" t="s">
         <v>18</v>
@@ -4346,7 +4353,7 @@
       </c>
       <c r="C56">
         <f>SUM(C48:C55)</f>
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4358,8 +4365,8 @@
         <v>193</v>
       </c>
       <c r="C57" s="6">
-        <f>SUM(C18,C28,C37,C46)</f>
-        <v>92</v>
+        <f>SUM(C18,C28,C37,C46,C56)</f>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -4372,7 +4379,7 @@
       </c>
       <c r="C58" s="53">
         <f>C57*100</f>
-        <v>9200</v>
+        <v>11500</v>
       </c>
       <c r="D58" s="53"/>
     </row>

</xml_diff>

<commit_message>
Updated Gantt to add my and Scott's changes
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\CS383\Tower-of-Annihilation\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sakur\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C95F1E4-9070-4D9B-9C5B-B58FC8E5FDAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDD8301-282D-4676-B6C9-0DEFC56424C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="264" yWindow="552" windowWidth="18816" windowHeight="11400" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Overhead" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="104">
   <si>
     <t>Total</t>
   </si>
@@ -348,6 +347,9 @@
   </si>
   <si>
     <t>Make player Static</t>
+  </si>
+  <si>
+    <t>Enemy Health Bar</t>
   </si>
 </sst>
 </file>
@@ -420,7 +422,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +474,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -620,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -700,6 +708,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -2252,31 +2263,31 @@
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="5.140625" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" customWidth="1"/>
+    <col min="18" max="18" width="5.109375" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="20" max="20" width="13.5546875" customWidth="1"/>
+    <col min="21" max="21" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C2" s="61" t="s">
         <v>0</v>
       </c>
@@ -2304,7 +2315,7 @@
       <c r="T2" s="62"/>
       <c r="U2" s="63"/>
     </row>
-    <row r="3" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
@@ -2352,7 +2363,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
         <v>8</v>
       </c>
@@ -2416,7 +2427,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
@@ -2426,11 +2437,11 @@
       </c>
       <c r="D5" s="18">
         <f t="shared" si="0"/>
-        <v>6300</v>
+        <v>7000</v>
       </c>
       <c r="E5" s="19">
         <f t="shared" ref="E5:E6" si="2">(C5-D5)</f>
-        <v>4300</v>
+        <v>3600</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="17">
@@ -2439,11 +2450,11 @@
       </c>
       <c r="H5" s="18">
         <f>(Gantt!$C28)*100</f>
-        <v>1800</v>
+        <v>2500</v>
       </c>
       <c r="I5" s="19">
         <f t="shared" ref="I5:I6" si="3">(G5-H5)</f>
-        <v>2700</v>
+        <v>2000</v>
       </c>
       <c r="K5" s="17">
         <v>2000</v>
@@ -2480,34 +2491,34 @@
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="17">
         <f t="shared" si="1"/>
-        <v>10900</v>
+        <v>10500</v>
       </c>
       <c r="D6" s="18">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>8600</v>
       </c>
       <c r="E6" s="19">
         <f t="shared" si="2"/>
-        <v>3400</v>
+        <v>1900</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="17">
-        <f>(Gantt!$B37)*100</f>
-        <v>4800</v>
+        <f>(Gantt!$B38)*100</f>
+        <v>4400</v>
       </c>
       <c r="H6" s="18">
-        <f>(Gantt!$C37)*100</f>
-        <v>2100</v>
+        <f>(Gantt!$C38)*100</f>
+        <v>3200</v>
       </c>
       <c r="I6" s="19">
         <f t="shared" si="3"/>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="K6" s="17">
         <v>2000</v>
@@ -2542,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
@@ -2560,11 +2571,11 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="17">
-        <f>(Gantt!$B46)*100</f>
+        <f>(Gantt!$B47)*100</f>
         <v>4900</v>
       </c>
       <c r="H7" s="18">
-        <f>(Gantt!$C46)*100</f>
+        <f>(Gantt!$C47)*100</f>
         <v>1300</v>
       </c>
       <c r="I7" s="19">
@@ -2606,7 +2617,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
@@ -2624,11 +2635,11 @@
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="17">
-        <f>(Gantt!$B56)*100</f>
+        <f>(Gantt!$B57)*100</f>
         <v>5700</v>
       </c>
       <c r="H8" s="18">
-        <f>(Gantt!$C56)*100</f>
+        <f>(Gantt!$C57)*100</f>
         <v>2300</v>
       </c>
       <c r="I8" s="19">
@@ -2670,34 +2681,34 @@
         <v>900</v>
       </c>
     </row>
-    <row r="9" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="27">
         <f>SUM(C4:C8)</f>
-        <v>55500</v>
+        <v>55100</v>
       </c>
       <c r="D9" s="28">
         <f>SUM(D4:D8)</f>
-        <v>34700</v>
+        <v>36500</v>
       </c>
       <c r="E9" s="29">
         <f>SUM(E4:E8)</f>
-        <v>20800</v>
+        <v>18600</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="20">
         <f>SUM(G4:G8)</f>
-        <v>25000</v>
+        <v>24600</v>
       </c>
       <c r="H9" s="21">
         <f>SUM(H4:H8)</f>
-        <v>11500</v>
+        <v>13300</v>
       </c>
       <c r="I9" s="22">
         <f>SUM(I4:I8)</f>
-        <v>13500</v>
+        <v>11300</v>
       </c>
       <c r="K9" s="20">
         <f>SUM(K4:K8)</f>
@@ -2751,22 +2762,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BK58"/>
+  <dimension ref="A1:BK59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" s="48"/>
       <c r="B1" s="48" t="s">
         <v>13</v>
@@ -2845,7 +2856,7 @@
       <c r="BJ1" s="48"/>
       <c r="BK1" s="48"/>
     </row>
-    <row r="2" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3107,7 +3118,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -3129,7 +3140,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3155,7 +3166,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3181,7 +3192,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3207,7 +3218,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="8" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3233,7 +3244,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3263,7 +3274,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>101</v>
       </c>
@@ -3277,7 +3288,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -3303,7 +3314,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -3329,7 +3340,7 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3355,7 +3366,7 @@
         <v>this week</v>
       </c>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -3377,7 +3388,7 @@
         <v>this week</v>
       </c>
     </row>
-    <row r="15" spans="1:63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -3388,7 +3399,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -3402,7 +3413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -3413,7 +3424,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -3426,19 +3437,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="65">
         <v>2</v>
       </c>
       <c r="D20" t="s">
@@ -3450,14 +3461,14 @@
       </c>
       <c r="F20" s="55"/>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="65">
         <v>5</v>
       </c>
       <c r="D21" t="s">
@@ -3471,14 +3482,14 @@
       <c r="G21" s="64"/>
       <c r="H21" s="64"/>
     </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="65">
         <v>2</v>
       </c>
       <c r="D22" t="s">
@@ -3497,15 +3508,15 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="23" spans="1:46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>36</v>
       </c>
       <c r="B23">
         <v>8</v>
       </c>
-      <c r="C23">
-        <v>3</v>
+      <c r="C23" s="65">
+        <v>4</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
@@ -3525,14 +3536,14 @@
       <c r="R23" s="64"/>
       <c r="S23" s="64"/>
     </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="65">
         <v>5</v>
       </c>
       <c r="D24" t="s">
@@ -3547,15 +3558,15 @@
       <c r="W24" s="64"/>
       <c r="X24" s="64"/>
     </row>
-    <row r="25" spans="1:46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
-      <c r="C25">
-        <v>1</v>
+      <c r="C25" s="65">
+        <v>7</v>
       </c>
       <c r="D25" t="s">
         <v>18</v>
@@ -3574,7 +3585,7 @@
       <c r="M25" s="64"/>
       <c r="N25" s="64"/>
     </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -3598,7 +3609,7 @@
       <c r="O26" s="64"/>
       <c r="P26" s="64"/>
     </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3631,7 +3642,7 @@
         <v>planned</v>
       </c>
     </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -3641,22 +3652,22 @@
       </c>
       <c r="C28">
         <f>SUM(C20:C27)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="65">
         <v>1</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="65">
         <v>1</v>
       </c>
       <c r="D30" t="s">
@@ -3667,14 +3678,14 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="65">
         <v>2</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="65">
         <v>3</v>
       </c>
       <c r="D31" t="s">
@@ -3693,14 +3704,14 @@
         <v>complete</v>
       </c>
     </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="65">
         <v>10</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="65">
         <v>9</v>
       </c>
       <c r="D32" t="s">
@@ -3738,15 +3749,18 @@
       <c r="Q32" s="55"/>
       <c r="R32" s="55"/>
     </row>
-    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>45</v>
       </c>
-      <c r="B33">
-        <v>5</v>
+      <c r="B33" s="65">
+        <v>6</v>
+      </c>
+      <c r="C33" s="65">
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="S33" s="60"/>
       <c r="T33" s="57"/>
@@ -3754,13 +3768,14 @@
       <c r="V33" s="57"/>
       <c r="W33" s="57"/>
     </row>
-    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="65">
         <v>5</v>
       </c>
+      <c r="C34" s="65"/>
       <c r="D34" t="s">
         <v>19</v>
       </c>
@@ -3770,15 +3785,15 @@
       <c r="AA34" s="57"/>
       <c r="AB34" s="57"/>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
-      <c r="B35">
-        <v>10</v>
-      </c>
-      <c r="C35">
-        <v>2</v>
+      <c r="B35" s="65">
+        <v>5</v>
+      </c>
+      <c r="C35" s="65">
+        <v>4</v>
       </c>
       <c r="D35" t="s">
         <v>18</v>
@@ -3799,91 +3814,87 @@
       <c r="AP35" s="3"/>
       <c r="AQ35" s="3"/>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B36">
-        <v>15</v>
-      </c>
-      <c r="C36">
-        <v>6</v>
+      <c r="B36" s="65">
+        <v>12</v>
+      </c>
+      <c r="C36" s="65">
+        <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM36" s="56"/>
-      <c r="AN36" s="56"/>
-      <c r="AO36" s="56"/>
-      <c r="AP36" s="56"/>
-      <c r="AQ36" s="56"/>
-      <c r="AR36" s="56"/>
-      <c r="AS36" s="56"/>
-      <c r="AT36" s="56"/>
-      <c r="AU36" s="56"/>
-      <c r="AV36" s="56"/>
-      <c r="AW36" s="56"/>
-      <c r="AX36" s="56"/>
-      <c r="AY36" s="56"/>
-      <c r="AZ36" s="56"/>
-      <c r="BA36" s="56"/>
+        <v>17</v>
+      </c>
+      <c r="AM36" s="67"/>
+      <c r="AN36" s="67"/>
+      <c r="AO36" s="67"/>
+      <c r="AP36" s="67"/>
+      <c r="AQ36" s="67"/>
+      <c r="AR36" s="67"/>
+      <c r="AS36" s="67"/>
+      <c r="AT36" s="67"/>
+      <c r="AU36" s="67"/>
+      <c r="AV36" s="67"/>
+      <c r="AW36" s="67"/>
+      <c r="AX36" s="67"/>
+      <c r="AY36" s="67"/>
+      <c r="AZ36" s="67"/>
+      <c r="BA36" s="67"/>
       <c r="BB36" s="3"/>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="65">
+        <v>3</v>
+      </c>
+      <c r="C37" s="65">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
+      <c r="AO37" s="3"/>
+      <c r="AP37" s="3"/>
+      <c r="AQ37" s="3"/>
+      <c r="AR37" s="3"/>
+      <c r="AS37" s="3"/>
+      <c r="AT37" s="3"/>
+      <c r="AU37" s="3"/>
+      <c r="AV37" s="3"/>
+      <c r="AW37" s="3"/>
+      <c r="AX37" s="3"/>
+      <c r="AY37" s="3"/>
+      <c r="AZ37" s="66"/>
+      <c r="BA37" s="66"/>
+      <c r="BB37" s="3"/>
+    </row>
+    <row r="38" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>32</v>
       </c>
-      <c r="B37">
-        <f>SUM(B30:B36)</f>
-        <v>48</v>
-      </c>
-      <c r="C37">
-        <f>SUM(C30:C36)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38">
+        <f>SUM(B30:B37)</f>
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <f>SUM(C30:C37)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>49</v>
-      </c>
-      <c r="B39">
-        <v>5</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" ref="E39:I39" si="12">($D39)</f>
-        <v>complete</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="12"/>
-        <v>complete</v>
-      </c>
-      <c r="G39" t="str">
-        <f t="shared" si="12"/>
-        <v>complete</v>
-      </c>
-      <c r="H39" t="str">
-        <f t="shared" si="12"/>
-        <v>complete</v>
-      </c>
-      <c r="I39" t="str">
-        <f t="shared" si="12"/>
-        <v>complete</v>
-      </c>
-    </row>
-    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>50</v>
       </c>
       <c r="B40">
         <v>5</v>
@@ -3894,494 +3905,528 @@
       <c r="D40" t="s">
         <v>17</v>
       </c>
-      <c r="J40" t="str">
-        <f t="shared" ref="J40:N40" si="13">($D40)</f>
-        <v>complete</v>
-      </c>
-      <c r="K40" t="str">
-        <f t="shared" si="13"/>
-        <v>complete</v>
-      </c>
-      <c r="L40" t="str">
-        <f t="shared" si="13"/>
-        <v>complete</v>
-      </c>
-      <c r="M40" t="str">
-        <f t="shared" si="13"/>
-        <v>complete</v>
-      </c>
-      <c r="N40" t="str">
-        <f t="shared" si="13"/>
-        <v>complete</v>
-      </c>
-    </row>
-    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="E40" t="str">
+        <f t="shared" ref="E40:I40" si="12">($D40)</f>
+        <v>complete</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="12"/>
+        <v>complete</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="12"/>
+        <v>complete</v>
+      </c>
+      <c r="H40" t="str">
+        <f t="shared" si="12"/>
+        <v>complete</v>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="12"/>
+        <v>complete</v>
+      </c>
+    </row>
+    <row r="41" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
       </c>
-      <c r="O41" t="str">
-        <f t="shared" ref="O41:T41" si="14">($D41)</f>
-        <v>complete</v>
-      </c>
-      <c r="P41" t="str">
+      <c r="J41" t="str">
+        <f t="shared" ref="J41:N41" si="13">($D41)</f>
+        <v>complete</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="13"/>
+        <v>complete</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="13"/>
+        <v>complete</v>
+      </c>
+      <c r="M41" t="str">
+        <f t="shared" si="13"/>
+        <v>complete</v>
+      </c>
+      <c r="N41" t="str">
+        <f t="shared" si="13"/>
+        <v>complete</v>
+      </c>
+    </row>
+    <row r="42" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" ref="O42:T42" si="14">($D42)</f>
+        <v>complete</v>
+      </c>
+      <c r="P42" t="str">
         <f t="shared" si="14"/>
         <v>complete</v>
       </c>
-      <c r="Q41" t="str">
+      <c r="Q42" t="str">
         <f t="shared" si="14"/>
         <v>complete</v>
       </c>
-      <c r="R41" t="str">
+      <c r="R42" t="str">
         <f t="shared" si="14"/>
         <v>complete</v>
       </c>
-      <c r="S41" t="str">
+      <c r="S42" t="str">
         <f t="shared" si="14"/>
         <v>complete</v>
       </c>
-      <c r="T41" t="str">
+      <c r="T42" t="str">
         <f t="shared" si="14"/>
         <v>complete</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>52</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>10</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>18</v>
       </c>
-      <c r="U42" t="str">
-        <f t="shared" ref="U42:V42" si="15">($D42)</f>
+      <c r="U43" t="str">
+        <f t="shared" ref="U43:V43" si="15">($D43)</f>
         <v>this week</v>
       </c>
-      <c r="V42" t="str">
+      <c r="V43" t="str">
         <f t="shared" si="15"/>
         <v>this week</v>
       </c>
     </row>
-    <row r="43" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>53</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>10</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>19</v>
       </c>
-      <c r="W43" t="str">
-        <f t="shared" ref="W43:AB43" si="16">($D43)</f>
+      <c r="W44" t="str">
+        <f t="shared" ref="W44:AB44" si="16">($D44)</f>
         <v>planned</v>
       </c>
-      <c r="X43" t="str">
+      <c r="X44" t="str">
         <f t="shared" si="16"/>
         <v>planned</v>
       </c>
-      <c r="Y43" t="str">
+      <c r="Y44" t="str">
         <f t="shared" si="16"/>
         <v>planned</v>
       </c>
-      <c r="Z43" t="str">
+      <c r="Z44" t="str">
         <f t="shared" si="16"/>
         <v>planned</v>
       </c>
-      <c r="AA43" t="str">
+      <c r="AA44" t="str">
         <f t="shared" si="16"/>
         <v>planned</v>
       </c>
-      <c r="AB43" t="str">
+      <c r="AB44" t="str">
         <f t="shared" si="16"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="44" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>10</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>19</v>
       </c>
-      <c r="AC44" t="str">
-        <f t="shared" ref="AC44:AD44" si="17">($D44)</f>
+      <c r="AC45" t="str">
+        <f t="shared" ref="AC45:AD45" si="17">($D45)</f>
         <v>planned</v>
       </c>
-      <c r="AD44" t="str">
+      <c r="AD45" t="str">
         <f t="shared" si="17"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="45" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>55</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>5</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>19</v>
       </c>
-      <c r="AE45" t="str">
-        <f t="shared" ref="AE45:AH45" si="18">($D45)</f>
+      <c r="AE46" t="str">
+        <f t="shared" ref="AE46:AH46" si="18">($D46)</f>
         <v>planned</v>
       </c>
-      <c r="AF45" t="str">
+      <c r="AF46" t="str">
         <f t="shared" si="18"/>
         <v>planned</v>
       </c>
-      <c r="AG45" t="str">
+      <c r="AG46" t="str">
         <f t="shared" si="18"/>
         <v>planned</v>
       </c>
-      <c r="AH45" t="str">
+      <c r="AH46" t="str">
         <f t="shared" si="18"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>32</v>
       </c>
-      <c r="B46">
-        <f>SUM(B39:B45)</f>
+      <c r="B47">
+        <f>SUM(B40:B46)</f>
         <v>49</v>
       </c>
-      <c r="C46">
-        <f>SUM(C39:C45)</f>
+      <c r="C47">
+        <f>SUM(C40:C46)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:54" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>10</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>7</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>17</v>
       </c>
-      <c r="E48" t="str">
-        <f t="shared" ref="E48:I48" si="19">($D48)</f>
-        <v>complete</v>
-      </c>
-      <c r="F48" t="str">
+      <c r="E49" t="str">
+        <f t="shared" ref="E49:I49" si="19">($D49)</f>
+        <v>complete</v>
+      </c>
+      <c r="F49" t="str">
         <f t="shared" si="19"/>
         <v>complete</v>
       </c>
-      <c r="G48" t="str">
+      <c r="G49" t="str">
         <f t="shared" si="19"/>
         <v>complete</v>
       </c>
-      <c r="H48" t="str">
+      <c r="H49" t="str">
         <f t="shared" si="19"/>
         <v>complete</v>
       </c>
-      <c r="I48" t="str">
+      <c r="I49" t="str">
         <f t="shared" si="19"/>
         <v>complete</v>
       </c>
-      <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-    </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
+    </row>
+    <row r="50" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>57</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>5</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <v>2</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>18</v>
       </c>
-      <c r="L49" t="str">
-        <f t="shared" ref="L49:P49" si="20">($D49)</f>
+      <c r="L50" t="str">
+        <f t="shared" ref="L50:P50" si="20">($D50)</f>
         <v>this week</v>
       </c>
-      <c r="M49" t="str">
+      <c r="M50" t="str">
         <f t="shared" si="20"/>
         <v>this week</v>
       </c>
-      <c r="N49" t="str">
+      <c r="N50" t="str">
         <f t="shared" si="20"/>
         <v>this week</v>
       </c>
-      <c r="O49" s="58" t="str">
-        <f>($D49)</f>
+      <c r="O50" s="58" t="str">
+        <f>($D50)</f>
         <v>this week</v>
       </c>
-      <c r="P49" s="3" t="str">
+      <c r="P50" s="3" t="str">
         <f t="shared" si="20"/>
         <v>this week</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>58</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>5</v>
       </c>
-      <c r="C50">
+      <c r="C51">
         <v>7</v>
       </c>
-      <c r="D50" s="56" t="s">
+      <c r="D51" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="Q50" t="str">
-        <f t="shared" ref="Q50:V50" si="21">($D50)</f>
+      <c r="Q51" t="str">
+        <f t="shared" ref="Q51:V51" si="21">($D51)</f>
         <v>this week</v>
       </c>
-      <c r="R50" t="str">
+      <c r="R51" t="str">
         <f t="shared" si="21"/>
         <v>this week</v>
       </c>
-      <c r="S50" t="str">
+      <c r="S51" t="str">
         <f t="shared" si="21"/>
         <v>this week</v>
       </c>
-      <c r="T50" t="str">
+      <c r="T51" t="str">
         <f t="shared" si="21"/>
         <v>this week</v>
       </c>
-      <c r="U50" t="str">
+      <c r="U51" t="str">
         <f t="shared" si="21"/>
         <v>this week</v>
       </c>
-      <c r="V50" t="str">
+      <c r="V51" t="str">
         <f t="shared" si="21"/>
         <v>this week</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>59</v>
-      </c>
-      <c r="B51">
-        <v>10</v>
-      </c>
-      <c r="C51">
-        <v>5</v>
-      </c>
-      <c r="D51" t="s">
-        <v>17</v>
-      </c>
-      <c r="W51" t="str">
-        <f t="shared" ref="W51:X51" si="22">($D51)</f>
-        <v>complete</v>
-      </c>
-      <c r="X51" t="str">
-        <f t="shared" si="22"/>
-        <v>complete</v>
-      </c>
-    </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>60</v>
       </c>
       <c r="B52">
         <v>10</v>
       </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
       <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="W52" t="str">
+        <f t="shared" ref="W52:X52" si="22">($D52)</f>
+        <v>complete</v>
+      </c>
+      <c r="X52" t="str">
+        <f t="shared" si="22"/>
+        <v>complete</v>
+      </c>
+    </row>
+    <row r="53" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
         <v>19</v>
       </c>
-      <c r="Y52" t="str">
-        <f t="shared" ref="Y52:AD52" si="23">($D52)</f>
+      <c r="Y53" t="str">
+        <f t="shared" ref="Y53:AD53" si="23">($D53)</f>
         <v>planned</v>
       </c>
-      <c r="Z52" t="str">
+      <c r="Z53" t="str">
         <f t="shared" si="23"/>
         <v>planned</v>
       </c>
-      <c r="AA52" t="str">
+      <c r="AA53" t="str">
         <f t="shared" si="23"/>
         <v>planned</v>
       </c>
-      <c r="AB52" t="str">
+      <c r="AB53" t="str">
         <f t="shared" si="23"/>
         <v>planned</v>
       </c>
-      <c r="AC52" t="str">
+      <c r="AC53" t="str">
         <f t="shared" si="23"/>
         <v>planned</v>
       </c>
-      <c r="AD52" t="str">
+      <c r="AD53" t="str">
         <f t="shared" si="23"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>61</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>10</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>19</v>
       </c>
-      <c r="AE53" t="str">
-        <f t="shared" ref="AE53:AJ53" si="24">($D53)</f>
+      <c r="AE54" t="str">
+        <f t="shared" ref="AE54:AJ54" si="24">($D54)</f>
         <v>planned</v>
       </c>
-      <c r="AF53" t="str">
+      <c r="AF54" t="str">
         <f t="shared" si="24"/>
         <v>planned</v>
       </c>
-      <c r="AG53" t="str">
+      <c r="AG54" t="str">
         <f t="shared" si="24"/>
         <v>planned</v>
       </c>
-      <c r="AH53" t="str">
+      <c r="AH54" t="str">
         <f t="shared" si="24"/>
         <v>planned</v>
       </c>
-      <c r="AI53" t="str">
+      <c r="AI54" t="str">
         <f t="shared" si="24"/>
         <v>planned</v>
       </c>
-      <c r="AJ53" t="str">
+      <c r="AJ54" t="str">
         <f t="shared" si="24"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>62</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>5</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <v>2</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>18</v>
       </c>
-      <c r="AK54" t="str">
-        <f t="shared" ref="AK54:AN54" si="25">($D54)</f>
+      <c r="AK55" t="str">
+        <f t="shared" ref="AK55:AN55" si="25">($D55)</f>
         <v>this week</v>
       </c>
-      <c r="AL54" t="str">
+      <c r="AL55" t="str">
         <f t="shared" si="25"/>
         <v>this week</v>
       </c>
-      <c r="AM54" t="str">
+      <c r="AM55" t="str">
         <f t="shared" si="25"/>
         <v>this week</v>
       </c>
-      <c r="AN54" t="str">
+      <c r="AN55" t="str">
         <f t="shared" si="25"/>
         <v>this week</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>63</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>2</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
-      <c r="Z55" s="3"/>
-      <c r="AA55" s="3"/>
-      <c r="AO55" t="str">
-        <f t="shared" ref="AO55:AP55" si="26">($D55)</f>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="3"/>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+      <c r="AA56" s="3"/>
+      <c r="AO56" t="str">
+        <f t="shared" ref="AO56:AP56" si="26">($D56)</f>
         <v>planned</v>
       </c>
-      <c r="AP55" t="str">
+      <c r="AP56" t="str">
         <f t="shared" si="26"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>32</v>
       </c>
-      <c r="B56">
-        <f>SUM(B48:B55)</f>
+      <c r="B57">
+        <f>SUM(B49:B56)</f>
         <v>57</v>
       </c>
-      <c r="C56">
-        <f>SUM(C48:C55)</f>
+      <c r="C57">
+        <f>SUM(C49:C56)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+    <row r="58" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="6">
-        <f>SUM(B37,B46,B28,B18)</f>
-        <v>193</v>
-      </c>
-      <c r="C57" s="6">
-        <f>SUM(C18,C28,C37,C46,C56)</f>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="B58" s="6">
+        <f>SUM(B38,B47,B28,B18)</f>
+        <v>189</v>
+      </c>
+      <c r="C58" s="6">
+        <f>SUM(C18,C28,C38,C47,C57)</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="53">
-        <f>B57*100</f>
-        <v>19300</v>
-      </c>
-      <c r="C58" s="53">
-        <f>C57*100</f>
-        <v>11500</v>
-      </c>
-      <c r="D58" s="53"/>
+      <c r="B59" s="53">
+        <f>B58*100</f>
+        <v>18900</v>
+      </c>
+      <c r="C59" s="53">
+        <f>C58*100</f>
+        <v>13300</v>
+      </c>
+      <c r="D59" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4392,7 +4437,7 @@
     <mergeCell ref="T24:X24"/>
     <mergeCell ref="G26:P26"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3 D20:D26 D48:D54">
+  <conditionalFormatting sqref="D3 D20:D26 D49:D55">
     <cfRule type="cellIs" dxfId="122" priority="178" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -4436,7 +4481,7 @@
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="D36:D37">
     <cfRule type="cellIs" dxfId="110" priority="166" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -4447,7 +4492,7 @@
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33:BR45 E32:O32 Q32:BR32 E22:BR22 E47:BR48 E49:I49 E50:J50 L49:BR49 L50:N50 Q50:BR50 E52:V52 E51:T51 E53:AJ53 Y52:AR52 W51:AR51 AW51:BR54 AM53:AR53 AQ54:AR54 E54:AN54 AO55:AP55 E28:BR31 E25 O25:BR25 I21:BR21 E21 E24:T24 E23:L23 T23:BR23 Y24:BR24 E26:G26 Q26:BR26 E27:Y27 AB27:BR27 E3:BR5 E6:I6 K6:BR6 E7:BR20">
+  <conditionalFormatting sqref="E33:BR36 E32:O32 Q32:BR32 E22:BR22 E48:BR49 E50:I50 E51:J51 L50:BR50 L51:N51 Q51:BR51 E53:V53 E52:T52 E54:AJ54 Y53:AR53 W52:AR52 AW52:BR55 AM54:AR54 AQ55:AR55 E55:AN55 AO56:AP56 E28:BR31 E25 O25:BR25 I21:BR21 E21 E24:T24 E23:L23 T23:BR23 Y24:BR24 E26:G26 Q26:BR26 E27:Y27 AB27:BR27 E3:BR5 E6:I6 K6:BR6 E7:BR20 E38:BR46 E37:AY37 BB37:BR37">
     <cfRule type="cellIs" dxfId="107" priority="160" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -4480,7 +4525,7 @@
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D45">
+  <conditionalFormatting sqref="D40:D46">
     <cfRule type="cellIs" dxfId="98" priority="148" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -4601,7 +4646,7 @@
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="cellIs" dxfId="65" priority="97" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -4844,7 +4889,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30:D36 D3:D17 D20:D27 D48:D55 D39:D45" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30:D37 D3:D17 D20:D27 D49:D56 D40:D46" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$F$1:$H$1</formula1>
     </dataValidation>
   </dataValidations>
@@ -4861,9 +4906,9 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>66</v>
       </c>
@@ -4892,7 +4937,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>67</v>
       </c>
@@ -4921,7 +4966,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>75</v>
       </c>
@@ -4950,7 +4995,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -4983,7 +5028,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -5016,7 +5061,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -5049,7 +5094,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -5082,7 +5127,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>12</v>
       </c>
@@ -5115,7 +5160,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
@@ -5164,15 +5209,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
   </sheetData>
@@ -5189,16 +5234,16 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="19" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="19" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="31"/>
       <c r="B1" s="32" t="s">
         <v>77</v>
@@ -5255,7 +5300,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>8</v>
       </c>
@@ -5271,7 +5316,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="46"/>
       <c r="B3" s="35" t="s">
         <v>81</v>
@@ -5288,7 +5333,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="38"/>
       <c r="B4" s="35" t="s">
         <v>82</v>
@@ -5304,7 +5349,7 @@
       <c r="I4" s="4"/>
       <c r="J4" s="52"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="38"/>
       <c r="B5" s="35" t="s">
         <v>83</v>
@@ -5318,7 +5363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
         <v>9</v>
       </c>
@@ -5334,7 +5379,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="46"/>
       <c r="B7" s="35" t="s">
         <v>81</v>
@@ -5351,7 +5396,7 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="38"/>
       <c r="B8" s="35" t="s">
         <v>84</v>
@@ -5367,7 +5412,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="47"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="38"/>
       <c r="B9" s="35" t="s">
         <v>83</v>
@@ -5381,7 +5426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>10</v>
       </c>
@@ -5396,7 +5441,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="46"/>
       <c r="B11" s="35" t="s">
         <v>81</v>
@@ -5413,7 +5458,7 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="38"/>
       <c r="B12" s="40" t="s">
         <v>85</v>
@@ -5429,7 +5474,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="38"/>
       <c r="B13" s="40" t="s">
         <v>87</v>
@@ -5444,7 +5489,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
       <c r="B14" s="40" t="s">
         <v>89</v>
@@ -5460,7 +5505,7 @@
       </c>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="38"/>
       <c r="B15" s="41" t="s">
         <v>83</v>
@@ -5474,7 +5519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>11</v>
       </c>
@@ -5490,7 +5535,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="46"/>
       <c r="B17" s="35" t="s">
         <v>81</v>
@@ -5507,7 +5552,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="38"/>
       <c r="B18" s="35" t="s">
         <v>91</v>
@@ -5523,7 +5568,7 @@
       <c r="I18" s="4"/>
       <c r="J18" s="47"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="38"/>
       <c r="B19" s="41" t="s">
         <v>83</v>
@@ -5537,7 +5582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="34" t="s">
         <v>12</v>
       </c>
@@ -5553,7 +5598,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="46"/>
       <c r="B21" s="35" t="s">
         <v>81</v>
@@ -5570,7 +5615,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="38"/>
       <c r="B22" s="35" t="s">
         <v>92</v>
@@ -5586,7 +5631,7 @@
       <c r="I22" s="4"/>
       <c r="J22" s="47"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="38"/>
       <c r="B23" s="41" t="s">
         <v>83</v>
@@ -5600,7 +5645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="42"/>
       <c r="B24" s="43" t="s">
         <v>0</v>
@@ -5614,7 +5659,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25" s="30" t="s">
         <v>93</v>
       </c>
@@ -5633,12 +5678,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="6" t="s">
         <v>8</v>
@@ -5656,7 +5701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>94</v>
       </c>
@@ -5676,7 +5721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>95</v>
       </c>
@@ -5696,7 +5741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>96</v>
       </c>
@@ -5716,7 +5761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>97</v>
       </c>
@@ -5736,20 +5781,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Small changes I forgot to push
 - Gantt chart chagnes
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\CS383\Tower-of-Annihilation\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2975CD-215E-428E-99DB-BAAE42EEDEB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C41D8-880C-4B57-B117-ED2045FAC2E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="106">
   <si>
     <t>Total</t>
   </si>
@@ -3768,28 +3768,28 @@
       </c>
       <c r="C8" s="17">
         <f t="shared" si="7"/>
-        <v>11800</v>
+        <v>12400</v>
       </c>
       <c r="D8" s="18">
         <f t="shared" si="8"/>
-        <v>6600</v>
+        <v>8100</v>
       </c>
       <c r="E8" s="19">
         <f t="shared" si="9"/>
-        <v>5200</v>
+        <v>4300</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="17">
-        <f>(Gantt!$B59)*100</f>
-        <v>5700</v>
+        <f>(Gantt!$B60)*100</f>
+        <v>6300</v>
       </c>
       <c r="H8" s="18">
-        <f>(Gantt!$C59)*100</f>
-        <v>2300</v>
+        <f>(Gantt!$C60)*100</f>
+        <v>3800</v>
       </c>
       <c r="I8" s="19">
         <f t="shared" si="10"/>
-        <v>3400</v>
+        <v>2500</v>
       </c>
       <c r="K8" s="17">
         <v>2000</v>
@@ -3832,28 +3832,28 @@
       </c>
       <c r="C9" s="27">
         <f>SUM(C4:C8)</f>
-        <v>56000</v>
+        <v>56600</v>
       </c>
       <c r="D9" s="28">
         <f>SUM(D4:D8)</f>
-        <v>37400</v>
+        <v>38900</v>
       </c>
       <c r="E9" s="29">
         <f>SUM(E4:E8)</f>
-        <v>18600</v>
+        <v>17700</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="20">
         <f>SUM(G4:G8)</f>
-        <v>25500</v>
+        <v>26100</v>
       </c>
       <c r="H9" s="21">
         <f>SUM(H4:H8)</f>
-        <v>14200</v>
+        <v>15700</v>
       </c>
       <c r="I9" s="22">
         <f>SUM(I4:I8)</f>
-        <v>11300</v>
+        <v>10400</v>
       </c>
       <c r="K9" s="20">
         <f>SUM(K4:K8)</f>
@@ -3907,10 +3907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BK61"/>
+  <dimension ref="A1:BK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5381,30 +5381,30 @@
         <v>5</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" ref="L52:P52" si="20">($D52)</f>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="M52" t="str">
         <f t="shared" si="20"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="20"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="O52" s="58" t="str">
         <f>($D52)</f>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="P52" s="3" t="str">
         <f t="shared" si="20"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
     </row>
     <row r="53" spans="1:42" x14ac:dyDescent="0.25">
@@ -5418,31 +5418,31 @@
         <v>7</v>
       </c>
       <c r="D53" s="56" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" ref="Q53:V53" si="21">($D53)</f>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="R53" t="str">
         <f t="shared" si="21"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="S53" t="str">
         <f t="shared" si="21"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="T53" t="str">
         <f t="shared" si="21"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="U53" t="str">
         <f t="shared" si="21"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
       <c r="V53" t="str">
         <f t="shared" si="21"/>
-        <v>this week</v>
+        <v>complete</v>
       </c>
     </row>
     <row r="54" spans="1:42" x14ac:dyDescent="0.25">
@@ -5545,7 +5545,7 @@
         <v>5</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
         <v>18</v>
@@ -5569,85 +5569,102 @@
     </row>
     <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+      <c r="C58">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>61</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>2</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>19</v>
       </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
-      <c r="Z58" s="3"/>
-      <c r="AA58" s="3"/>
-      <c r="AO58" t="str">
-        <f t="shared" ref="AO58:AP58" si="26">($D58)</f>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="3"/>
+      <c r="U59" s="3"/>
+      <c r="V59" s="3"/>
+      <c r="W59" s="3"/>
+      <c r="X59" s="3"/>
+      <c r="Y59" s="3"/>
+      <c r="Z59" s="3"/>
+      <c r="AA59" s="3"/>
+      <c r="AO59" t="str">
+        <f t="shared" ref="AO59:AP59" si="26">($D59)</f>
         <v>planned</v>
       </c>
-      <c r="AP58" t="str">
+      <c r="AP59" t="str">
         <f t="shared" si="26"/>
         <v>planned</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>31</v>
       </c>
-      <c r="B59">
-        <f>SUM(B51:B58)</f>
-        <v>57</v>
-      </c>
-      <c r="C59">
-        <f>SUM(C51:C58)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="60" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="B60">
+        <f>SUM(B51:B59)</f>
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <f>SUM(C51:C59)</f>
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B60" s="6">
+      <c r="B61" s="6">
         <f>SUM(B40,B49,B30,B20)</f>
         <v>198</v>
       </c>
-      <c r="C60" s="6">
-        <f>SUM(C20,C30,C40,C49,C59)</f>
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="C61" s="6">
+        <f>SUM(C20,C30,C40,C49,C60)</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:42" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="53">
-        <f>B60*100</f>
+      <c r="B62" s="53">
+        <f>B61*100</f>
         <v>19800</v>
       </c>
-      <c r="C61" s="53">
-        <f>C60*100</f>
-        <v>14200</v>
-      </c>
-      <c r="D61" s="53"/>
+      <c r="C62" s="53">
+        <f>C61*100</f>
+        <v>15700</v>
+      </c>
+      <c r="D62" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5658,7 +5675,7 @@
     <mergeCell ref="T26:X26"/>
     <mergeCell ref="G28:P28"/>
   </mergeCells>
-  <conditionalFormatting sqref="D3 D22:D28 D51:D57">
+  <conditionalFormatting sqref="D3 D22:D28 D51:D58 D60">
     <cfRule type="cellIs" dxfId="236" priority="292" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -5713,7 +5730,7 @@
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35:BR38 E34:O34 Q34:BR34 E24:BR24 E50:BR51 E52:I52 E53:J53 L52:BR52 L53:N53 Q53:BR53 E55:V55 E54:T54 E56:AJ56 Y55:AR55 W54:AR54 AW54:BR57 AM56:AR56 AQ57:AR57 E57:AN57 AO58:AP58 E30:BR33 E27 O27:BR27 I23:BR23 E23 E26:T26 E25:L25 T25:BR25 Y26:BR26 E28:G28 Q28:BR28 E29:Y29 AB29:BR29 E3:BR5 E6:I6 K6:BR6 E40:BR48 E39:AY39 BB39:BR39 E7:BR14 E18:BR18 E20:BR22">
+  <conditionalFormatting sqref="E35:BR38 E34:O34 Q34:BR34 E24:BR24 E50:BR51 E52:I52 E53:J53 L52:BR52 L53:N53 Q53:BR53 E55:V55 E54:T54 E56:AJ56 Y55:AR55 W54:AR54 AW54:BR58 AM56:AR56 AQ57:AR58 E57:AN58 AO59:AP59 E30:BR33 E27 O27:BR27 I23:BR23 E23 E26:T26 E25:L25 T25:BR25 Y26:BR26 E28:G28 Q28:BR28 E29:Y29 AB29:BR29 E3:BR5 E6:I6 K6:BR6 E40:BR48 E39:AY39 BB39:BR39 E7:BR14 E18:BR18 E20:BR22">
     <cfRule type="cellIs" dxfId="221" priority="274" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -5867,7 +5884,7 @@
       <formula>$F$1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
+  <conditionalFormatting sqref="D59">
     <cfRule type="cellIs" dxfId="179" priority="211" operator="equal">
       <formula>$H$1</formula>
     </cfRule>
@@ -6528,7 +6545,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D32:D39 D42:D48 D22:D29 D51:D58 D3:D19" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D32:D39 D42:D48 D22:D29 D51:D59 D3:D19" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$F$1:$H$1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>